<commit_message>
reverse linked list by recursive way modified
</commit_message>
<xml_diff>
--- a/DSA_A2Z/src/com/FINAL450.xlsx
+++ b/DSA_A2Z/src/com/FINAL450.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Learning\Java\DSA\DSA_A2Z\DSA_A2Z\src\com\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E1A487-8ED1-4299-8C3C-DC099DC15689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15195" windowHeight="6930"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1353" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1353" uniqueCount="468">
   <si>
     <t>Topic:</t>
   </si>
@@ -1420,13 +1426,16 @@
   </si>
   <si>
     <t>SR.NO</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1502,6 +1511,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1530,7 +1553,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1554,7 +1577,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1564,6 +1587,13 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1871,29 +1901,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F482"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
-      <selection activeCell="C129" sqref="C129"/>
+    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
+      <selection activeCell="D141" sqref="D141"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="15.6"/>
   <cols>
     <col min="2" max="2" width="28.5" customWidth="1"/>
     <col min="3" max="3" width="123" customWidth="1"/>
     <col min="4" max="4" width="27.5" customWidth="1"/>
-    <col min="6" max="6" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="26.25">
+    <row r="1" spans="1:6" ht="24.6">
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:6">
@@ -1962,7 +1992,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="19.5">
+    <row r="9" spans="1:6" ht="19.8">
       <c r="A9">
         <v>4</v>
       </c>
@@ -3579,7 +3609,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="21">
+    <row r="129" spans="1:5" ht="21">
       <c r="A129">
         <v>118</v>
       </c>
@@ -3593,7 +3623,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="21">
+    <row r="130" spans="1:5" ht="21">
       <c r="A130">
         <v>119</v>
       </c>
@@ -3607,7 +3637,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="21">
+    <row r="131" spans="1:5" ht="21">
       <c r="A131">
         <v>120</v>
       </c>
@@ -3621,7 +3651,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="21">
+    <row r="132" spans="1:5" ht="21">
       <c r="A132">
         <v>121</v>
       </c>
@@ -3635,7 +3665,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="21">
+    <row r="133" spans="1:5" ht="21">
       <c r="A133">
         <v>122</v>
       </c>
@@ -3649,7 +3679,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="134" spans="1:4" ht="21">
+    <row r="134" spans="1:5" ht="21">
       <c r="A134">
         <v>123</v>
       </c>
@@ -3663,7 +3693,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="21">
+    <row r="135" spans="1:5" ht="21">
       <c r="A135">
         <v>124</v>
       </c>
@@ -3677,7 +3707,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="21">
+    <row r="136" spans="1:5" ht="21">
       <c r="A136">
         <v>125</v>
       </c>
@@ -3691,7 +3721,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="21">
+    <row r="137" spans="1:5" ht="21">
       <c r="A137">
         <v>126</v>
       </c>
@@ -3705,33 +3735,39 @@
         <v>3</v>
       </c>
     </row>
-    <row r="139" spans="1:4" ht="21">
+    <row r="139" spans="1:5" ht="21">
       <c r="C139" s="7"/>
       <c r="D139" s="4"/>
     </row>
-    <row r="140" spans="1:4" ht="21">
+    <row r="140" spans="1:5" ht="21">
       <c r="B140" s="8" t="s">
         <v>133</v>
       </c>
       <c r="C140" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="D140" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" ht="21">
+      <c r="D140" s="16" t="s">
+        <v>467</v>
+      </c>
+      <c r="E140" s="17">
+        <v>45739</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" ht="21">
       <c r="B141" s="8" t="s">
         <v>133</v>
       </c>
       <c r="C141" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="D141" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" ht="21">
+      <c r="D141" s="15" t="s">
+        <v>467</v>
+      </c>
+      <c r="E141" s="17">
+        <v>45739</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" ht="21">
       <c r="B142" s="8" t="s">
         <v>133</v>
       </c>
@@ -3742,7 +3778,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="21">
+    <row r="143" spans="1:5" ht="21">
       <c r="B143" s="8" t="s">
         <v>133</v>
       </c>
@@ -3753,7 +3789,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="21">
+    <row r="144" spans="1:5" ht="21">
       <c r="B144" s="8" t="s">
         <v>133</v>
       </c>
@@ -7343,452 +7379,452 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C6" r:id="rId1"/>
-    <hyperlink ref="C7" r:id="rId2"/>
-    <hyperlink ref="C8" r:id="rId3"/>
-    <hyperlink ref="C10" r:id="rId4"/>
-    <hyperlink ref="C11" r:id="rId5"/>
-    <hyperlink ref="C12" r:id="rId6"/>
-    <hyperlink ref="C13" r:id="rId7"/>
-    <hyperlink ref="C14" r:id="rId8"/>
-    <hyperlink ref="C15" r:id="rId9"/>
-    <hyperlink ref="C16" r:id="rId10"/>
-    <hyperlink ref="C17" r:id="rId11"/>
-    <hyperlink ref="C18" r:id="rId12"/>
-    <hyperlink ref="C19" r:id="rId13"/>
-    <hyperlink ref="C20" r:id="rId14"/>
-    <hyperlink ref="C21" r:id="rId15"/>
-    <hyperlink ref="C22" r:id="rId16"/>
-    <hyperlink ref="C23" r:id="rId17"/>
-    <hyperlink ref="C24" r:id="rId18"/>
-    <hyperlink ref="C25" r:id="rId19"/>
-    <hyperlink ref="C26" r:id="rId20"/>
-    <hyperlink ref="C27" r:id="rId21"/>
-    <hyperlink ref="C28" r:id="rId22"/>
-    <hyperlink ref="C29" r:id="rId23"/>
-    <hyperlink ref="C30" r:id="rId24"/>
-    <hyperlink ref="C31" r:id="rId25"/>
-    <hyperlink ref="C32" r:id="rId26"/>
-    <hyperlink ref="C33" r:id="rId27"/>
-    <hyperlink ref="C34" r:id="rId28"/>
-    <hyperlink ref="C35" r:id="rId29"/>
-    <hyperlink ref="C36" r:id="rId30"/>
-    <hyperlink ref="C37" r:id="rId31"/>
-    <hyperlink ref="C38" r:id="rId32"/>
-    <hyperlink ref="C39" r:id="rId33"/>
-    <hyperlink ref="C40" r:id="rId34"/>
-    <hyperlink ref="C41" r:id="rId35"/>
-    <hyperlink ref="C42" r:id="rId36"/>
-    <hyperlink ref="C45" r:id="rId37"/>
-    <hyperlink ref="C46" r:id="rId38"/>
-    <hyperlink ref="C47" r:id="rId39"/>
-    <hyperlink ref="C48" r:id="rId40"/>
-    <hyperlink ref="C49" r:id="rId41"/>
-    <hyperlink ref="C50" r:id="rId42"/>
-    <hyperlink ref="C51" r:id="rId43"/>
-    <hyperlink ref="C52" r:id="rId44"/>
-    <hyperlink ref="C53" r:id="rId45"/>
-    <hyperlink ref="C54" r:id="rId46"/>
-    <hyperlink ref="C57" r:id="rId47"/>
-    <hyperlink ref="C58" r:id="rId48"/>
-    <hyperlink ref="C59" r:id="rId49"/>
-    <hyperlink ref="C61" r:id="rId50"/>
-    <hyperlink ref="C62" r:id="rId51"/>
-    <hyperlink ref="C63" r:id="rId52"/>
-    <hyperlink ref="C64" r:id="rId53"/>
-    <hyperlink ref="C65" r:id="rId54"/>
-    <hyperlink ref="C66" r:id="rId55"/>
-    <hyperlink ref="C67" r:id="rId56"/>
-    <hyperlink ref="C68" r:id="rId57"/>
-    <hyperlink ref="C69" r:id="rId58"/>
-    <hyperlink ref="C70" r:id="rId59"/>
-    <hyperlink ref="C71" r:id="rId60"/>
-    <hyperlink ref="C72" r:id="rId61"/>
-    <hyperlink ref="C73" r:id="rId62"/>
-    <hyperlink ref="C74" r:id="rId63"/>
-    <hyperlink ref="C75" r:id="rId64"/>
-    <hyperlink ref="C76" r:id="rId65"/>
-    <hyperlink ref="C77" r:id="rId66"/>
-    <hyperlink ref="C78" r:id="rId67"/>
-    <hyperlink ref="C79" r:id="rId68"/>
-    <hyperlink ref="C80" r:id="rId69"/>
-    <hyperlink ref="C81" r:id="rId70"/>
-    <hyperlink ref="C82" r:id="rId71"/>
-    <hyperlink ref="C83" r:id="rId72"/>
-    <hyperlink ref="C84" r:id="rId73"/>
-    <hyperlink ref="C85" r:id="rId74"/>
-    <hyperlink ref="C86" r:id="rId75"/>
-    <hyperlink ref="C87" r:id="rId76"/>
-    <hyperlink ref="C88" r:id="rId77"/>
-    <hyperlink ref="C89" r:id="rId78"/>
-    <hyperlink ref="C90" r:id="rId79"/>
-    <hyperlink ref="C91" r:id="rId80"/>
-    <hyperlink ref="C92" r:id="rId81"/>
-    <hyperlink ref="C93" r:id="rId82"/>
-    <hyperlink ref="C94" r:id="rId83"/>
-    <hyperlink ref="C95" r:id="rId84"/>
-    <hyperlink ref="C96" r:id="rId85"/>
-    <hyperlink ref="C97" r:id="rId86"/>
-    <hyperlink ref="C98" r:id="rId87"/>
-    <hyperlink ref="C99" r:id="rId88"/>
-    <hyperlink ref="C102" r:id="rId89"/>
-    <hyperlink ref="C103" r:id="rId90"/>
-    <hyperlink ref="C104" r:id="rId91"/>
-    <hyperlink ref="C105" r:id="rId92"/>
-    <hyperlink ref="C107" r:id="rId93" location=":~:text=We%20need%20to%20find%20a,set%20of%20points%20is%20minimum.&amp;text=In%20above%20figure%20optimum%20location,is%20minimum%20obtainable%20total%20distance."/>
-    <hyperlink ref="C108" r:id="rId94"/>
-    <hyperlink ref="C109" r:id="rId95"/>
-    <hyperlink ref="C110" r:id="rId96"/>
-    <hyperlink ref="C111" r:id="rId97"/>
-    <hyperlink ref="C112" r:id="rId98"/>
-    <hyperlink ref="C114" r:id="rId99"/>
-    <hyperlink ref="C115" r:id="rId100"/>
-    <hyperlink ref="C116" r:id="rId101"/>
-    <hyperlink ref="C117" r:id="rId102"/>
-    <hyperlink ref="C118" r:id="rId103"/>
-    <hyperlink ref="C119" r:id="rId104"/>
-    <hyperlink ref="C120" r:id="rId105"/>
-    <hyperlink ref="C121" r:id="rId106"/>
-    <hyperlink ref="C122" r:id="rId107"/>
-    <hyperlink ref="C123" r:id="rId108"/>
-    <hyperlink ref="C124" r:id="rId109"/>
-    <hyperlink ref="C125" r:id="rId110"/>
-    <hyperlink ref="C126" r:id="rId111"/>
-    <hyperlink ref="C127" r:id="rId112"/>
-    <hyperlink ref="C128" r:id="rId113"/>
-    <hyperlink ref="C129" r:id="rId114"/>
-    <hyperlink ref="C130" r:id="rId115"/>
-    <hyperlink ref="C131" r:id="rId116"/>
-    <hyperlink ref="C132" r:id="rId117"/>
-    <hyperlink ref="C133" r:id="rId118"/>
-    <hyperlink ref="C134" r:id="rId119"/>
-    <hyperlink ref="C135" r:id="rId120"/>
-    <hyperlink ref="C136" r:id="rId121"/>
-    <hyperlink ref="C137" r:id="rId122"/>
-    <hyperlink ref="C106" r:id="rId123"/>
-    <hyperlink ref="C113" r:id="rId124"/>
-    <hyperlink ref="C140" r:id="rId125"/>
-    <hyperlink ref="C141" r:id="rId126"/>
-    <hyperlink ref="C142" r:id="rId127"/>
-    <hyperlink ref="C143" r:id="rId128"/>
-    <hyperlink ref="C144" r:id="rId129"/>
-    <hyperlink ref="C145" r:id="rId130"/>
-    <hyperlink ref="C146" r:id="rId131"/>
-    <hyperlink ref="C147" r:id="rId132"/>
-    <hyperlink ref="C148" r:id="rId133"/>
-    <hyperlink ref="C149" r:id="rId134"/>
-    <hyperlink ref="C150" r:id="rId135"/>
-    <hyperlink ref="C151" r:id="rId136"/>
-    <hyperlink ref="C152" r:id="rId137"/>
-    <hyperlink ref="C153" r:id="rId138"/>
-    <hyperlink ref="C154" r:id="rId139"/>
-    <hyperlink ref="C155" r:id="rId140"/>
-    <hyperlink ref="C156" r:id="rId141"/>
-    <hyperlink ref="C157" r:id="rId142"/>
-    <hyperlink ref="C158" r:id="rId143"/>
-    <hyperlink ref="C159" r:id="rId144"/>
-    <hyperlink ref="C160" r:id="rId145"/>
-    <hyperlink ref="C161" r:id="rId146"/>
-    <hyperlink ref="C162" r:id="rId147"/>
-    <hyperlink ref="C163" r:id="rId148"/>
-    <hyperlink ref="C164" r:id="rId149"/>
-    <hyperlink ref="C167" r:id="rId150"/>
-    <hyperlink ref="C168" r:id="rId151"/>
-    <hyperlink ref="C169" r:id="rId152"/>
-    <hyperlink ref="C170" r:id="rId153"/>
-    <hyperlink ref="C171" r:id="rId154"/>
-    <hyperlink ref="C172" r:id="rId155"/>
-    <hyperlink ref="C173" r:id="rId156"/>
-    <hyperlink ref="C174" r:id="rId157"/>
-    <hyperlink ref="C175" r:id="rId158"/>
-    <hyperlink ref="C178" r:id="rId159"/>
-    <hyperlink ref="C179" r:id="rId160"/>
-    <hyperlink ref="C180" r:id="rId161"/>
-    <hyperlink ref="C181" r:id="rId162"/>
-    <hyperlink ref="C182" r:id="rId163"/>
-    <hyperlink ref="C183" r:id="rId164"/>
-    <hyperlink ref="C184" r:id="rId165"/>
-    <hyperlink ref="C185" r:id="rId166"/>
-    <hyperlink ref="C186" r:id="rId167"/>
-    <hyperlink ref="C187" r:id="rId168"/>
-    <hyperlink ref="C188" r:id="rId169"/>
-    <hyperlink ref="C189" r:id="rId170"/>
-    <hyperlink ref="C190" r:id="rId171"/>
-    <hyperlink ref="C191" r:id="rId172"/>
-    <hyperlink ref="C192" r:id="rId173"/>
-    <hyperlink ref="C193" r:id="rId174"/>
-    <hyperlink ref="C194" r:id="rId175"/>
-    <hyperlink ref="C195" r:id="rId176"/>
-    <hyperlink ref="C196" r:id="rId177"/>
-    <hyperlink ref="C197" r:id="rId178"/>
-    <hyperlink ref="C198" r:id="rId179" location=":~:text=Given%20the%20array%20representation%20of,it%20into%20Binary%20Search%20Tree.&amp;text=Swap%201%3A%20Swap%20node%208,node%209%20with%20node%2010."/>
-    <hyperlink ref="C199" r:id="rId180"/>
-    <hyperlink ref="C200" r:id="rId181"/>
-    <hyperlink ref="C201" r:id="rId182"/>
-    <hyperlink ref="C202" r:id="rId183"/>
-    <hyperlink ref="C203" r:id="rId184"/>
-    <hyperlink ref="C204" r:id="rId185" location=":~:text=Since%20the%20graph%20is%20undirected,graph%20is%20connected%2C%20otherwise%20not."/>
-    <hyperlink ref="C205" r:id="rId186"/>
-    <hyperlink ref="C206" r:id="rId187"/>
-    <hyperlink ref="C207" r:id="rId188"/>
-    <hyperlink ref="C208" r:id="rId189"/>
-    <hyperlink ref="C209" r:id="rId190"/>
-    <hyperlink ref="C210" r:id="rId191"/>
-    <hyperlink ref="C211" r:id="rId192"/>
-    <hyperlink ref="C212" r:id="rId193"/>
-    <hyperlink ref="C215" r:id="rId194"/>
-    <hyperlink ref="C216" r:id="rId195"/>
-    <hyperlink ref="C217" r:id="rId196"/>
-    <hyperlink ref="C218" r:id="rId197"/>
-    <hyperlink ref="C219" r:id="rId198"/>
-    <hyperlink ref="C220" r:id="rId199"/>
-    <hyperlink ref="C221" r:id="rId200"/>
-    <hyperlink ref="C222" r:id="rId201"/>
-    <hyperlink ref="C223" r:id="rId202"/>
-    <hyperlink ref="C224" r:id="rId203"/>
-    <hyperlink ref="C225" r:id="rId204"/>
-    <hyperlink ref="C226" r:id="rId205"/>
-    <hyperlink ref="C227" r:id="rId206"/>
-    <hyperlink ref="C228" r:id="rId207"/>
-    <hyperlink ref="C229" r:id="rId208"/>
-    <hyperlink ref="C230" r:id="rId209"/>
-    <hyperlink ref="C231" r:id="rId210"/>
-    <hyperlink ref="C232" r:id="rId211"/>
-    <hyperlink ref="C233" r:id="rId212"/>
-    <hyperlink ref="C234" r:id="rId213"/>
-    <hyperlink ref="C235" r:id="rId214"/>
-    <hyperlink ref="C236" r:id="rId215"/>
-    <hyperlink ref="C239" r:id="rId216"/>
-    <hyperlink ref="C240" r:id="rId217"/>
-    <hyperlink ref="C241" r:id="rId218"/>
-    <hyperlink ref="C242" r:id="rId219"/>
-    <hyperlink ref="C243" r:id="rId220"/>
-    <hyperlink ref="C244" r:id="rId221"/>
-    <hyperlink ref="C245" r:id="rId222"/>
-    <hyperlink ref="C246" r:id="rId223"/>
-    <hyperlink ref="C247" r:id="rId224"/>
-    <hyperlink ref="C248" r:id="rId225"/>
-    <hyperlink ref="C249" r:id="rId226"/>
-    <hyperlink ref="C250" r:id="rId227"/>
-    <hyperlink ref="C251" r:id="rId228"/>
-    <hyperlink ref="C252" r:id="rId229"/>
-    <hyperlink ref="C253" r:id="rId230"/>
-    <hyperlink ref="C254" r:id="rId231"/>
-    <hyperlink ref="C255" r:id="rId232"/>
-    <hyperlink ref="C256" r:id="rId233"/>
-    <hyperlink ref="C257" r:id="rId234"/>
-    <hyperlink ref="C258" r:id="rId235" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S."/>
-    <hyperlink ref="C259" r:id="rId236"/>
-    <hyperlink ref="C260" r:id="rId237"/>
-    <hyperlink ref="C261" r:id="rId238"/>
-    <hyperlink ref="C262" r:id="rId239"/>
-    <hyperlink ref="C263" r:id="rId240"/>
-    <hyperlink ref="C264" r:id="rId241"/>
-    <hyperlink ref="C265" r:id="rId242"/>
-    <hyperlink ref="C266" r:id="rId243"/>
-    <hyperlink ref="C267" r:id="rId244"/>
-    <hyperlink ref="C268" r:id="rId245"/>
-    <hyperlink ref="C269" r:id="rId246"/>
-    <hyperlink ref="C270" r:id="rId247"/>
-    <hyperlink ref="C271" r:id="rId248"/>
-    <hyperlink ref="C272" r:id="rId249"/>
-    <hyperlink ref="C273" r:id="rId250"/>
-    <hyperlink ref="C276" r:id="rId251"/>
-    <hyperlink ref="C277" r:id="rId252"/>
-    <hyperlink ref="C278" r:id="rId253"/>
-    <hyperlink ref="C279" r:id="rId254"/>
-    <hyperlink ref="C280" r:id="rId255"/>
-    <hyperlink ref="C281" r:id="rId256"/>
-    <hyperlink ref="C282" r:id="rId257"/>
-    <hyperlink ref="C283" r:id="rId258"/>
-    <hyperlink ref="C284" r:id="rId259"/>
-    <hyperlink ref="C285" r:id="rId260"/>
-    <hyperlink ref="C286" r:id="rId261"/>
-    <hyperlink ref="C287" r:id="rId262"/>
-    <hyperlink ref="C288" r:id="rId263"/>
-    <hyperlink ref="C289" r:id="rId264"/>
-    <hyperlink ref="C290" r:id="rId265"/>
-    <hyperlink ref="C291" r:id="rId266"/>
-    <hyperlink ref="C292" r:id="rId267"/>
-    <hyperlink ref="C293" r:id="rId268"/>
-    <hyperlink ref="C294" r:id="rId269"/>
-    <hyperlink ref="C297" r:id="rId270"/>
-    <hyperlink ref="C298" r:id="rId271"/>
-    <hyperlink ref="C299" r:id="rId272"/>
-    <hyperlink ref="C300" r:id="rId273"/>
-    <hyperlink ref="C301" r:id="rId274"/>
-    <hyperlink ref="C302" r:id="rId275"/>
-    <hyperlink ref="C303" r:id="rId276"/>
-    <hyperlink ref="C304" r:id="rId277"/>
-    <hyperlink ref="C305" r:id="rId278"/>
-    <hyperlink ref="C306" r:id="rId279"/>
-    <hyperlink ref="C307" r:id="rId280" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)."/>
-    <hyperlink ref="C308" r:id="rId281"/>
-    <hyperlink ref="C309" r:id="rId282"/>
-    <hyperlink ref="C310" r:id="rId283"/>
-    <hyperlink ref="C311" r:id="rId284"/>
-    <hyperlink ref="C312" r:id="rId285"/>
-    <hyperlink ref="C313" r:id="rId286"/>
-    <hyperlink ref="C314" r:id="rId287"/>
-    <hyperlink ref="C315" r:id="rId288"/>
-    <hyperlink ref="C316" r:id="rId289"/>
-    <hyperlink ref="C317" r:id="rId290"/>
-    <hyperlink ref="C318" r:id="rId291"/>
-    <hyperlink ref="C319" r:id="rId292"/>
-    <hyperlink ref="C320" r:id="rId293"/>
-    <hyperlink ref="C321" r:id="rId294"/>
-    <hyperlink ref="C322" r:id="rId295"/>
-    <hyperlink ref="C323" r:id="rId296"/>
-    <hyperlink ref="C324" r:id="rId297"/>
-    <hyperlink ref="C325" r:id="rId298"/>
-    <hyperlink ref="C326" r:id="rId299"/>
-    <hyperlink ref="C327" r:id="rId300"/>
-    <hyperlink ref="C328" r:id="rId301"/>
-    <hyperlink ref="C329" r:id="rId302"/>
-    <hyperlink ref="C330" r:id="rId303"/>
-    <hyperlink ref="C331" r:id="rId304"/>
-    <hyperlink ref="C332" r:id="rId305"/>
-    <hyperlink ref="C333" r:id="rId306"/>
-    <hyperlink ref="C334" r:id="rId307"/>
-    <hyperlink ref="C337" r:id="rId308"/>
-    <hyperlink ref="C338" r:id="rId309"/>
-    <hyperlink ref="C339" r:id="rId310"/>
-    <hyperlink ref="C340" r:id="rId311"/>
-    <hyperlink ref="C341" r:id="rId312"/>
-    <hyperlink ref="C342" r:id="rId313"/>
-    <hyperlink ref="C343" r:id="rId314"/>
-    <hyperlink ref="C344" r:id="rId315"/>
-    <hyperlink ref="C345" r:id="rId316"/>
-    <hyperlink ref="C346" r:id="rId317"/>
-    <hyperlink ref="C347" r:id="rId318"/>
-    <hyperlink ref="C348" r:id="rId319"/>
-    <hyperlink ref="C349" r:id="rId320"/>
-    <hyperlink ref="C350" r:id="rId321"/>
-    <hyperlink ref="C351" r:id="rId322"/>
-    <hyperlink ref="C352" r:id="rId323"/>
-    <hyperlink ref="C353" r:id="rId324"/>
-    <hyperlink ref="C354" r:id="rId325"/>
-    <hyperlink ref="C358" r:id="rId326"/>
-    <hyperlink ref="C359" r:id="rId327"/>
-    <hyperlink ref="C360" r:id="rId328"/>
-    <hyperlink ref="C361" r:id="rId329"/>
-    <hyperlink ref="C362" r:id="rId330"/>
-    <hyperlink ref="C363" r:id="rId331"/>
-    <hyperlink ref="C364" r:id="rId332"/>
-    <hyperlink ref="C365" r:id="rId333"/>
-    <hyperlink ref="C366" r:id="rId334"/>
-    <hyperlink ref="C367" r:id="rId335"/>
-    <hyperlink ref="C368" r:id="rId336"/>
-    <hyperlink ref="C369" r:id="rId337"/>
-    <hyperlink ref="C370" r:id="rId338"/>
-    <hyperlink ref="C371" r:id="rId339"/>
-    <hyperlink ref="C372" r:id="rId340"/>
-    <hyperlink ref="C373" r:id="rId341"/>
-    <hyperlink ref="C374" r:id="rId342"/>
-    <hyperlink ref="C375" r:id="rId343"/>
-    <hyperlink ref="C376" r:id="rId344"/>
-    <hyperlink ref="C377" r:id="rId345"/>
-    <hyperlink ref="C378" r:id="rId346"/>
-    <hyperlink ref="C379" r:id="rId347"/>
-    <hyperlink ref="C380" r:id="rId348" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color."/>
-    <hyperlink ref="C381" r:id="rId349"/>
-    <hyperlink ref="C382" r:id="rId350"/>
-    <hyperlink ref="C383" r:id="rId351"/>
-    <hyperlink ref="C384" r:id="rId352"/>
-    <hyperlink ref="C385" r:id="rId353"/>
-    <hyperlink ref="C386" r:id="rId354"/>
-    <hyperlink ref="C387" r:id="rId355"/>
-    <hyperlink ref="C388" r:id="rId356"/>
-    <hyperlink ref="C389" r:id="rId357"/>
-    <hyperlink ref="C390" r:id="rId358"/>
-    <hyperlink ref="C391" r:id="rId359"/>
-    <hyperlink ref="C392" r:id="rId360"/>
-    <hyperlink ref="C393" r:id="rId361"/>
-    <hyperlink ref="C394" r:id="rId362"/>
-    <hyperlink ref="C395" r:id="rId363"/>
-    <hyperlink ref="C397" r:id="rId364"/>
-    <hyperlink ref="C396" r:id="rId365"/>
-    <hyperlink ref="C398" r:id="rId366"/>
-    <hyperlink ref="C399" r:id="rId367"/>
-    <hyperlink ref="C400" r:id="rId368"/>
-    <hyperlink ref="C403" r:id="rId369"/>
-    <hyperlink ref="C404" r:id="rId370"/>
-    <hyperlink ref="C405" r:id="rId371"/>
-    <hyperlink ref="C406" r:id="rId372"/>
-    <hyperlink ref="C407" r:id="rId373"/>
-    <hyperlink ref="C408" r:id="rId374"/>
-    <hyperlink ref="C411" r:id="rId375"/>
-    <hyperlink ref="C412" r:id="rId376"/>
-    <hyperlink ref="C413" r:id="rId377"/>
-    <hyperlink ref="C414" r:id="rId378"/>
-    <hyperlink ref="C415" r:id="rId379"/>
-    <hyperlink ref="C416" r:id="rId380"/>
-    <hyperlink ref="C417" r:id="rId381"/>
-    <hyperlink ref="C418" r:id="rId382"/>
-    <hyperlink ref="C419" r:id="rId383"/>
-    <hyperlink ref="C420" r:id="rId384"/>
-    <hyperlink ref="C421" r:id="rId385"/>
-    <hyperlink ref="C422" r:id="rId386"/>
-    <hyperlink ref="C423" r:id="rId387"/>
-    <hyperlink ref="C424" r:id="rId388"/>
-    <hyperlink ref="C425" r:id="rId389"/>
-    <hyperlink ref="C426" r:id="rId390"/>
-    <hyperlink ref="C427" r:id="rId391"/>
-    <hyperlink ref="C428" r:id="rId392"/>
-    <hyperlink ref="C429" r:id="rId393"/>
-    <hyperlink ref="C430" r:id="rId394"/>
-    <hyperlink ref="C431" r:id="rId395"/>
-    <hyperlink ref="C432" r:id="rId396"/>
-    <hyperlink ref="C433" r:id="rId397"/>
-    <hyperlink ref="C434" r:id="rId398"/>
-    <hyperlink ref="C435" r:id="rId399"/>
-    <hyperlink ref="C436" r:id="rId400"/>
-    <hyperlink ref="C437" r:id="rId401"/>
-    <hyperlink ref="C438" r:id="rId402"/>
-    <hyperlink ref="C439" r:id="rId403"/>
-    <hyperlink ref="C440" r:id="rId404"/>
-    <hyperlink ref="C441" r:id="rId405"/>
-    <hyperlink ref="C442" r:id="rId406"/>
-    <hyperlink ref="C443" r:id="rId407"/>
-    <hyperlink ref="C444" r:id="rId408"/>
-    <hyperlink ref="C445" r:id="rId409"/>
-    <hyperlink ref="C446" r:id="rId410"/>
-    <hyperlink ref="C447" r:id="rId411"/>
-    <hyperlink ref="C448" r:id="rId412"/>
-    <hyperlink ref="C449" r:id="rId413"/>
-    <hyperlink ref="C450" r:id="rId414"/>
-    <hyperlink ref="C452" r:id="rId415"/>
-    <hyperlink ref="C451" r:id="rId416"/>
-    <hyperlink ref="C453" r:id="rId417"/>
-    <hyperlink ref="C454" r:id="rId418"/>
-    <hyperlink ref="C455" r:id="rId419"/>
-    <hyperlink ref="C456" r:id="rId420"/>
-    <hyperlink ref="C457" r:id="rId421"/>
-    <hyperlink ref="C458" r:id="rId422"/>
-    <hyperlink ref="C459" r:id="rId423"/>
-    <hyperlink ref="C460" r:id="rId424"/>
-    <hyperlink ref="C461" r:id="rId425"/>
-    <hyperlink ref="C462" r:id="rId426"/>
-    <hyperlink ref="C463" r:id="rId427"/>
-    <hyperlink ref="C470" r:id="rId428"/>
-    <hyperlink ref="C469" r:id="rId429"/>
-    <hyperlink ref="C468" r:id="rId430"/>
-    <hyperlink ref="C467" r:id="rId431"/>
-    <hyperlink ref="C466" r:id="rId432"/>
-    <hyperlink ref="C465" r:id="rId433"/>
-    <hyperlink ref="C464" r:id="rId434"/>
-    <hyperlink ref="C473" r:id="rId435"/>
-    <hyperlink ref="C474" r:id="rId436"/>
-    <hyperlink ref="C475" r:id="rId437"/>
-    <hyperlink ref="C476" r:id="rId438"/>
-    <hyperlink ref="C477" r:id="rId439"/>
-    <hyperlink ref="C478" r:id="rId440"/>
-    <hyperlink ref="C479" r:id="rId441"/>
-    <hyperlink ref="C482" r:id="rId442"/>
-    <hyperlink ref="C480" r:id="rId443"/>
-    <hyperlink ref="C481" r:id="rId444" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result."/>
-    <hyperlink ref="C357" r:id="rId445"/>
-    <hyperlink ref="C9" r:id="rId446"/>
+    <hyperlink ref="C6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C7" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C8" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C10" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C11" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C12" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C13" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="C14" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="C15" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="C16" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="C17" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="C18" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="C19" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="C20" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="C21" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="C22" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="C23" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="C24" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="C25" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="C26" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="C27" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="C28" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="C29" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="C30" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="C31" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="C32" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="C33" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="C34" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="C35" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="C36" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="C37" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="C38" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="C39" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="C40" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="C41" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="C42" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="C45" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="C46" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="C47" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="C48" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="C49" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="C50" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="C51" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="C52" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="C53" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="C54" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="C57" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="C58" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="C59" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="C61" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="C62" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="C63" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="C64" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="C65" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="C66" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="C67" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="C68" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="C69" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="C70" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="C71" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="C72" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="C73" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="C74" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="C75" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="C76" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="C77" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="C78" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="C79" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="C80" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="C81" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="C82" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="C83" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="C84" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="C85" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="C86" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="C87" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="C88" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="C89" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="C90" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="C91" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="C92" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="C93" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="C94" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="C95" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="C96" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="C97" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="C98" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="C99" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="C102" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="C103" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="C104" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="C105" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="C107" r:id="rId93" location=":~:text=We%20need%20to%20find%20a,set%20of%20points%20is%20minimum.&amp;text=In%20above%20figure%20optimum%20location,is%20minimum%20obtainable%20total%20distance." xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="C108" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="C109" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="C110" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="C111" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="C112" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="C114" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="C115" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="C116" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="C117" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="C118" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="C119" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="C120" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
+    <hyperlink ref="C121" r:id="rId106" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="C122" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="C123" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="C124" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="C125" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="C126" r:id="rId111" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="C127" r:id="rId112" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="C128" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
+    <hyperlink ref="C129" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="C130" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="C131" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="C132" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="C133" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
+    <hyperlink ref="C134" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
+    <hyperlink ref="C135" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
+    <hyperlink ref="C136" r:id="rId121" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
+    <hyperlink ref="C137" r:id="rId122" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
+    <hyperlink ref="C106" r:id="rId123" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
+    <hyperlink ref="C113" r:id="rId124" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
+    <hyperlink ref="C140" r:id="rId125" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
+    <hyperlink ref="C141" r:id="rId126" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
+    <hyperlink ref="C142" r:id="rId127" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
+    <hyperlink ref="C143" r:id="rId128" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
+    <hyperlink ref="C144" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
+    <hyperlink ref="C145" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
+    <hyperlink ref="C146" r:id="rId131" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
+    <hyperlink ref="C147" r:id="rId132" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
+    <hyperlink ref="C148" r:id="rId133" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
+    <hyperlink ref="C149" r:id="rId134" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
+    <hyperlink ref="C150" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
+    <hyperlink ref="C151" r:id="rId136" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
+    <hyperlink ref="C152" r:id="rId137" xr:uid="{00000000-0004-0000-0000-000088000000}"/>
+    <hyperlink ref="C153" r:id="rId138" xr:uid="{00000000-0004-0000-0000-000089000000}"/>
+    <hyperlink ref="C154" r:id="rId139" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
+    <hyperlink ref="C155" r:id="rId140" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
+    <hyperlink ref="C156" r:id="rId141" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
+    <hyperlink ref="C157" r:id="rId142" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
+    <hyperlink ref="C158" r:id="rId143" xr:uid="{00000000-0004-0000-0000-00008E000000}"/>
+    <hyperlink ref="C159" r:id="rId144" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
+    <hyperlink ref="C160" r:id="rId145" xr:uid="{00000000-0004-0000-0000-000090000000}"/>
+    <hyperlink ref="C161" r:id="rId146" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
+    <hyperlink ref="C162" r:id="rId147" xr:uid="{00000000-0004-0000-0000-000092000000}"/>
+    <hyperlink ref="C163" r:id="rId148" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
+    <hyperlink ref="C164" r:id="rId149" xr:uid="{00000000-0004-0000-0000-000094000000}"/>
+    <hyperlink ref="C167" r:id="rId150" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
+    <hyperlink ref="C168" r:id="rId151" xr:uid="{00000000-0004-0000-0000-000096000000}"/>
+    <hyperlink ref="C169" r:id="rId152" xr:uid="{00000000-0004-0000-0000-000097000000}"/>
+    <hyperlink ref="C170" r:id="rId153" xr:uid="{00000000-0004-0000-0000-000098000000}"/>
+    <hyperlink ref="C171" r:id="rId154" xr:uid="{00000000-0004-0000-0000-000099000000}"/>
+    <hyperlink ref="C172" r:id="rId155" xr:uid="{00000000-0004-0000-0000-00009A000000}"/>
+    <hyperlink ref="C173" r:id="rId156" xr:uid="{00000000-0004-0000-0000-00009B000000}"/>
+    <hyperlink ref="C174" r:id="rId157" xr:uid="{00000000-0004-0000-0000-00009C000000}"/>
+    <hyperlink ref="C175" r:id="rId158" xr:uid="{00000000-0004-0000-0000-00009D000000}"/>
+    <hyperlink ref="C178" r:id="rId159" xr:uid="{00000000-0004-0000-0000-00009E000000}"/>
+    <hyperlink ref="C179" r:id="rId160" xr:uid="{00000000-0004-0000-0000-00009F000000}"/>
+    <hyperlink ref="C180" r:id="rId161" xr:uid="{00000000-0004-0000-0000-0000A0000000}"/>
+    <hyperlink ref="C181" r:id="rId162" xr:uid="{00000000-0004-0000-0000-0000A1000000}"/>
+    <hyperlink ref="C182" r:id="rId163" xr:uid="{00000000-0004-0000-0000-0000A2000000}"/>
+    <hyperlink ref="C183" r:id="rId164" xr:uid="{00000000-0004-0000-0000-0000A3000000}"/>
+    <hyperlink ref="C184" r:id="rId165" xr:uid="{00000000-0004-0000-0000-0000A4000000}"/>
+    <hyperlink ref="C185" r:id="rId166" xr:uid="{00000000-0004-0000-0000-0000A5000000}"/>
+    <hyperlink ref="C186" r:id="rId167" xr:uid="{00000000-0004-0000-0000-0000A6000000}"/>
+    <hyperlink ref="C187" r:id="rId168" xr:uid="{00000000-0004-0000-0000-0000A7000000}"/>
+    <hyperlink ref="C188" r:id="rId169" xr:uid="{00000000-0004-0000-0000-0000A8000000}"/>
+    <hyperlink ref="C189" r:id="rId170" xr:uid="{00000000-0004-0000-0000-0000A9000000}"/>
+    <hyperlink ref="C190" r:id="rId171" xr:uid="{00000000-0004-0000-0000-0000AA000000}"/>
+    <hyperlink ref="C191" r:id="rId172" xr:uid="{00000000-0004-0000-0000-0000AB000000}"/>
+    <hyperlink ref="C192" r:id="rId173" xr:uid="{00000000-0004-0000-0000-0000AC000000}"/>
+    <hyperlink ref="C193" r:id="rId174" xr:uid="{00000000-0004-0000-0000-0000AD000000}"/>
+    <hyperlink ref="C194" r:id="rId175" xr:uid="{00000000-0004-0000-0000-0000AE000000}"/>
+    <hyperlink ref="C195" r:id="rId176" xr:uid="{00000000-0004-0000-0000-0000AF000000}"/>
+    <hyperlink ref="C196" r:id="rId177" xr:uid="{00000000-0004-0000-0000-0000B0000000}"/>
+    <hyperlink ref="C197" r:id="rId178" xr:uid="{00000000-0004-0000-0000-0000B1000000}"/>
+    <hyperlink ref="C198" r:id="rId179" location=":~:text=Given%20the%20array%20representation%20of,it%20into%20Binary%20Search%20Tree.&amp;text=Swap%201%3A%20Swap%20node%208,node%209%20with%20node%2010." xr:uid="{00000000-0004-0000-0000-0000B2000000}"/>
+    <hyperlink ref="C199" r:id="rId180" xr:uid="{00000000-0004-0000-0000-0000B3000000}"/>
+    <hyperlink ref="C200" r:id="rId181" xr:uid="{00000000-0004-0000-0000-0000B4000000}"/>
+    <hyperlink ref="C201" r:id="rId182" xr:uid="{00000000-0004-0000-0000-0000B5000000}"/>
+    <hyperlink ref="C202" r:id="rId183" xr:uid="{00000000-0004-0000-0000-0000B6000000}"/>
+    <hyperlink ref="C203" r:id="rId184" xr:uid="{00000000-0004-0000-0000-0000B7000000}"/>
+    <hyperlink ref="C204" r:id="rId185" location=":~:text=Since%20the%20graph%20is%20undirected,graph%20is%20connected%2C%20otherwise%20not." xr:uid="{00000000-0004-0000-0000-0000B8000000}"/>
+    <hyperlink ref="C205" r:id="rId186" xr:uid="{00000000-0004-0000-0000-0000B9000000}"/>
+    <hyperlink ref="C206" r:id="rId187" xr:uid="{00000000-0004-0000-0000-0000BA000000}"/>
+    <hyperlink ref="C207" r:id="rId188" xr:uid="{00000000-0004-0000-0000-0000BB000000}"/>
+    <hyperlink ref="C208" r:id="rId189" xr:uid="{00000000-0004-0000-0000-0000BC000000}"/>
+    <hyperlink ref="C209" r:id="rId190" xr:uid="{00000000-0004-0000-0000-0000BD000000}"/>
+    <hyperlink ref="C210" r:id="rId191" xr:uid="{00000000-0004-0000-0000-0000BE000000}"/>
+    <hyperlink ref="C211" r:id="rId192" xr:uid="{00000000-0004-0000-0000-0000BF000000}"/>
+    <hyperlink ref="C212" r:id="rId193" xr:uid="{00000000-0004-0000-0000-0000C0000000}"/>
+    <hyperlink ref="C215" r:id="rId194" xr:uid="{00000000-0004-0000-0000-0000C1000000}"/>
+    <hyperlink ref="C216" r:id="rId195" xr:uid="{00000000-0004-0000-0000-0000C2000000}"/>
+    <hyperlink ref="C217" r:id="rId196" xr:uid="{00000000-0004-0000-0000-0000C3000000}"/>
+    <hyperlink ref="C218" r:id="rId197" xr:uid="{00000000-0004-0000-0000-0000C4000000}"/>
+    <hyperlink ref="C219" r:id="rId198" xr:uid="{00000000-0004-0000-0000-0000C5000000}"/>
+    <hyperlink ref="C220" r:id="rId199" xr:uid="{00000000-0004-0000-0000-0000C6000000}"/>
+    <hyperlink ref="C221" r:id="rId200" xr:uid="{00000000-0004-0000-0000-0000C7000000}"/>
+    <hyperlink ref="C222" r:id="rId201" xr:uid="{00000000-0004-0000-0000-0000C8000000}"/>
+    <hyperlink ref="C223" r:id="rId202" xr:uid="{00000000-0004-0000-0000-0000C9000000}"/>
+    <hyperlink ref="C224" r:id="rId203" xr:uid="{00000000-0004-0000-0000-0000CA000000}"/>
+    <hyperlink ref="C225" r:id="rId204" xr:uid="{00000000-0004-0000-0000-0000CB000000}"/>
+    <hyperlink ref="C226" r:id="rId205" xr:uid="{00000000-0004-0000-0000-0000CC000000}"/>
+    <hyperlink ref="C227" r:id="rId206" xr:uid="{00000000-0004-0000-0000-0000CD000000}"/>
+    <hyperlink ref="C228" r:id="rId207" xr:uid="{00000000-0004-0000-0000-0000CE000000}"/>
+    <hyperlink ref="C229" r:id="rId208" xr:uid="{00000000-0004-0000-0000-0000CF000000}"/>
+    <hyperlink ref="C230" r:id="rId209" xr:uid="{00000000-0004-0000-0000-0000D0000000}"/>
+    <hyperlink ref="C231" r:id="rId210" xr:uid="{00000000-0004-0000-0000-0000D1000000}"/>
+    <hyperlink ref="C232" r:id="rId211" xr:uid="{00000000-0004-0000-0000-0000D2000000}"/>
+    <hyperlink ref="C233" r:id="rId212" xr:uid="{00000000-0004-0000-0000-0000D3000000}"/>
+    <hyperlink ref="C234" r:id="rId213" xr:uid="{00000000-0004-0000-0000-0000D4000000}"/>
+    <hyperlink ref="C235" r:id="rId214" xr:uid="{00000000-0004-0000-0000-0000D5000000}"/>
+    <hyperlink ref="C236" r:id="rId215" xr:uid="{00000000-0004-0000-0000-0000D6000000}"/>
+    <hyperlink ref="C239" r:id="rId216" xr:uid="{00000000-0004-0000-0000-0000D7000000}"/>
+    <hyperlink ref="C240" r:id="rId217" xr:uid="{00000000-0004-0000-0000-0000D8000000}"/>
+    <hyperlink ref="C241" r:id="rId218" xr:uid="{00000000-0004-0000-0000-0000D9000000}"/>
+    <hyperlink ref="C242" r:id="rId219" xr:uid="{00000000-0004-0000-0000-0000DA000000}"/>
+    <hyperlink ref="C243" r:id="rId220" xr:uid="{00000000-0004-0000-0000-0000DB000000}"/>
+    <hyperlink ref="C244" r:id="rId221" xr:uid="{00000000-0004-0000-0000-0000DC000000}"/>
+    <hyperlink ref="C245" r:id="rId222" xr:uid="{00000000-0004-0000-0000-0000DD000000}"/>
+    <hyperlink ref="C246" r:id="rId223" xr:uid="{00000000-0004-0000-0000-0000DE000000}"/>
+    <hyperlink ref="C247" r:id="rId224" xr:uid="{00000000-0004-0000-0000-0000DF000000}"/>
+    <hyperlink ref="C248" r:id="rId225" xr:uid="{00000000-0004-0000-0000-0000E0000000}"/>
+    <hyperlink ref="C249" r:id="rId226" xr:uid="{00000000-0004-0000-0000-0000E1000000}"/>
+    <hyperlink ref="C250" r:id="rId227" xr:uid="{00000000-0004-0000-0000-0000E2000000}"/>
+    <hyperlink ref="C251" r:id="rId228" xr:uid="{00000000-0004-0000-0000-0000E3000000}"/>
+    <hyperlink ref="C252" r:id="rId229" xr:uid="{00000000-0004-0000-0000-0000E4000000}"/>
+    <hyperlink ref="C253" r:id="rId230" xr:uid="{00000000-0004-0000-0000-0000E5000000}"/>
+    <hyperlink ref="C254" r:id="rId231" xr:uid="{00000000-0004-0000-0000-0000E6000000}"/>
+    <hyperlink ref="C255" r:id="rId232" xr:uid="{00000000-0004-0000-0000-0000E7000000}"/>
+    <hyperlink ref="C256" r:id="rId233" xr:uid="{00000000-0004-0000-0000-0000E8000000}"/>
+    <hyperlink ref="C257" r:id="rId234" xr:uid="{00000000-0004-0000-0000-0000E9000000}"/>
+    <hyperlink ref="C258" r:id="rId235" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S." xr:uid="{00000000-0004-0000-0000-0000EA000000}"/>
+    <hyperlink ref="C259" r:id="rId236" xr:uid="{00000000-0004-0000-0000-0000EB000000}"/>
+    <hyperlink ref="C260" r:id="rId237" xr:uid="{00000000-0004-0000-0000-0000EC000000}"/>
+    <hyperlink ref="C261" r:id="rId238" xr:uid="{00000000-0004-0000-0000-0000ED000000}"/>
+    <hyperlink ref="C262" r:id="rId239" xr:uid="{00000000-0004-0000-0000-0000EE000000}"/>
+    <hyperlink ref="C263" r:id="rId240" xr:uid="{00000000-0004-0000-0000-0000EF000000}"/>
+    <hyperlink ref="C264" r:id="rId241" xr:uid="{00000000-0004-0000-0000-0000F0000000}"/>
+    <hyperlink ref="C265" r:id="rId242" xr:uid="{00000000-0004-0000-0000-0000F1000000}"/>
+    <hyperlink ref="C266" r:id="rId243" xr:uid="{00000000-0004-0000-0000-0000F2000000}"/>
+    <hyperlink ref="C267" r:id="rId244" xr:uid="{00000000-0004-0000-0000-0000F3000000}"/>
+    <hyperlink ref="C268" r:id="rId245" xr:uid="{00000000-0004-0000-0000-0000F4000000}"/>
+    <hyperlink ref="C269" r:id="rId246" xr:uid="{00000000-0004-0000-0000-0000F5000000}"/>
+    <hyperlink ref="C270" r:id="rId247" xr:uid="{00000000-0004-0000-0000-0000F6000000}"/>
+    <hyperlink ref="C271" r:id="rId248" xr:uid="{00000000-0004-0000-0000-0000F7000000}"/>
+    <hyperlink ref="C272" r:id="rId249" xr:uid="{00000000-0004-0000-0000-0000F8000000}"/>
+    <hyperlink ref="C273" r:id="rId250" xr:uid="{00000000-0004-0000-0000-0000F9000000}"/>
+    <hyperlink ref="C276" r:id="rId251" xr:uid="{00000000-0004-0000-0000-0000FA000000}"/>
+    <hyperlink ref="C277" r:id="rId252" xr:uid="{00000000-0004-0000-0000-0000FB000000}"/>
+    <hyperlink ref="C278" r:id="rId253" xr:uid="{00000000-0004-0000-0000-0000FC000000}"/>
+    <hyperlink ref="C279" r:id="rId254" xr:uid="{00000000-0004-0000-0000-0000FD000000}"/>
+    <hyperlink ref="C280" r:id="rId255" xr:uid="{00000000-0004-0000-0000-0000FE000000}"/>
+    <hyperlink ref="C281" r:id="rId256" xr:uid="{00000000-0004-0000-0000-0000FF000000}"/>
+    <hyperlink ref="C282" r:id="rId257" xr:uid="{00000000-0004-0000-0000-000000010000}"/>
+    <hyperlink ref="C283" r:id="rId258" xr:uid="{00000000-0004-0000-0000-000001010000}"/>
+    <hyperlink ref="C284" r:id="rId259" xr:uid="{00000000-0004-0000-0000-000002010000}"/>
+    <hyperlink ref="C285" r:id="rId260" xr:uid="{00000000-0004-0000-0000-000003010000}"/>
+    <hyperlink ref="C286" r:id="rId261" xr:uid="{00000000-0004-0000-0000-000004010000}"/>
+    <hyperlink ref="C287" r:id="rId262" xr:uid="{00000000-0004-0000-0000-000005010000}"/>
+    <hyperlink ref="C288" r:id="rId263" xr:uid="{00000000-0004-0000-0000-000006010000}"/>
+    <hyperlink ref="C289" r:id="rId264" xr:uid="{00000000-0004-0000-0000-000007010000}"/>
+    <hyperlink ref="C290" r:id="rId265" xr:uid="{00000000-0004-0000-0000-000008010000}"/>
+    <hyperlink ref="C291" r:id="rId266" xr:uid="{00000000-0004-0000-0000-000009010000}"/>
+    <hyperlink ref="C292" r:id="rId267" xr:uid="{00000000-0004-0000-0000-00000A010000}"/>
+    <hyperlink ref="C293" r:id="rId268" xr:uid="{00000000-0004-0000-0000-00000B010000}"/>
+    <hyperlink ref="C294" r:id="rId269" xr:uid="{00000000-0004-0000-0000-00000C010000}"/>
+    <hyperlink ref="C297" r:id="rId270" xr:uid="{00000000-0004-0000-0000-00000D010000}"/>
+    <hyperlink ref="C298" r:id="rId271" xr:uid="{00000000-0004-0000-0000-00000E010000}"/>
+    <hyperlink ref="C299" r:id="rId272" xr:uid="{00000000-0004-0000-0000-00000F010000}"/>
+    <hyperlink ref="C300" r:id="rId273" xr:uid="{00000000-0004-0000-0000-000010010000}"/>
+    <hyperlink ref="C301" r:id="rId274" xr:uid="{00000000-0004-0000-0000-000011010000}"/>
+    <hyperlink ref="C302" r:id="rId275" xr:uid="{00000000-0004-0000-0000-000012010000}"/>
+    <hyperlink ref="C303" r:id="rId276" xr:uid="{00000000-0004-0000-0000-000013010000}"/>
+    <hyperlink ref="C304" r:id="rId277" xr:uid="{00000000-0004-0000-0000-000014010000}"/>
+    <hyperlink ref="C305" r:id="rId278" xr:uid="{00000000-0004-0000-0000-000015010000}"/>
+    <hyperlink ref="C306" r:id="rId279" xr:uid="{00000000-0004-0000-0000-000016010000}"/>
+    <hyperlink ref="C307" r:id="rId280" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)." xr:uid="{00000000-0004-0000-0000-000017010000}"/>
+    <hyperlink ref="C308" r:id="rId281" xr:uid="{00000000-0004-0000-0000-000018010000}"/>
+    <hyperlink ref="C309" r:id="rId282" xr:uid="{00000000-0004-0000-0000-000019010000}"/>
+    <hyperlink ref="C310" r:id="rId283" xr:uid="{00000000-0004-0000-0000-00001A010000}"/>
+    <hyperlink ref="C311" r:id="rId284" xr:uid="{00000000-0004-0000-0000-00001B010000}"/>
+    <hyperlink ref="C312" r:id="rId285" xr:uid="{00000000-0004-0000-0000-00001C010000}"/>
+    <hyperlink ref="C313" r:id="rId286" xr:uid="{00000000-0004-0000-0000-00001D010000}"/>
+    <hyperlink ref="C314" r:id="rId287" xr:uid="{00000000-0004-0000-0000-00001E010000}"/>
+    <hyperlink ref="C315" r:id="rId288" xr:uid="{00000000-0004-0000-0000-00001F010000}"/>
+    <hyperlink ref="C316" r:id="rId289" xr:uid="{00000000-0004-0000-0000-000020010000}"/>
+    <hyperlink ref="C317" r:id="rId290" xr:uid="{00000000-0004-0000-0000-000021010000}"/>
+    <hyperlink ref="C318" r:id="rId291" xr:uid="{00000000-0004-0000-0000-000022010000}"/>
+    <hyperlink ref="C319" r:id="rId292" xr:uid="{00000000-0004-0000-0000-000023010000}"/>
+    <hyperlink ref="C320" r:id="rId293" xr:uid="{00000000-0004-0000-0000-000024010000}"/>
+    <hyperlink ref="C321" r:id="rId294" xr:uid="{00000000-0004-0000-0000-000025010000}"/>
+    <hyperlink ref="C322" r:id="rId295" xr:uid="{00000000-0004-0000-0000-000026010000}"/>
+    <hyperlink ref="C323" r:id="rId296" xr:uid="{00000000-0004-0000-0000-000027010000}"/>
+    <hyperlink ref="C324" r:id="rId297" xr:uid="{00000000-0004-0000-0000-000028010000}"/>
+    <hyperlink ref="C325" r:id="rId298" xr:uid="{00000000-0004-0000-0000-000029010000}"/>
+    <hyperlink ref="C326" r:id="rId299" xr:uid="{00000000-0004-0000-0000-00002A010000}"/>
+    <hyperlink ref="C327" r:id="rId300" xr:uid="{00000000-0004-0000-0000-00002B010000}"/>
+    <hyperlink ref="C328" r:id="rId301" xr:uid="{00000000-0004-0000-0000-00002C010000}"/>
+    <hyperlink ref="C329" r:id="rId302" xr:uid="{00000000-0004-0000-0000-00002D010000}"/>
+    <hyperlink ref="C330" r:id="rId303" xr:uid="{00000000-0004-0000-0000-00002E010000}"/>
+    <hyperlink ref="C331" r:id="rId304" xr:uid="{00000000-0004-0000-0000-00002F010000}"/>
+    <hyperlink ref="C332" r:id="rId305" xr:uid="{00000000-0004-0000-0000-000030010000}"/>
+    <hyperlink ref="C333" r:id="rId306" xr:uid="{00000000-0004-0000-0000-000031010000}"/>
+    <hyperlink ref="C334" r:id="rId307" xr:uid="{00000000-0004-0000-0000-000032010000}"/>
+    <hyperlink ref="C337" r:id="rId308" xr:uid="{00000000-0004-0000-0000-000033010000}"/>
+    <hyperlink ref="C338" r:id="rId309" xr:uid="{00000000-0004-0000-0000-000034010000}"/>
+    <hyperlink ref="C339" r:id="rId310" xr:uid="{00000000-0004-0000-0000-000035010000}"/>
+    <hyperlink ref="C340" r:id="rId311" xr:uid="{00000000-0004-0000-0000-000036010000}"/>
+    <hyperlink ref="C341" r:id="rId312" xr:uid="{00000000-0004-0000-0000-000037010000}"/>
+    <hyperlink ref="C342" r:id="rId313" xr:uid="{00000000-0004-0000-0000-000038010000}"/>
+    <hyperlink ref="C343" r:id="rId314" xr:uid="{00000000-0004-0000-0000-000039010000}"/>
+    <hyperlink ref="C344" r:id="rId315" xr:uid="{00000000-0004-0000-0000-00003A010000}"/>
+    <hyperlink ref="C345" r:id="rId316" xr:uid="{00000000-0004-0000-0000-00003B010000}"/>
+    <hyperlink ref="C346" r:id="rId317" xr:uid="{00000000-0004-0000-0000-00003C010000}"/>
+    <hyperlink ref="C347" r:id="rId318" xr:uid="{00000000-0004-0000-0000-00003D010000}"/>
+    <hyperlink ref="C348" r:id="rId319" xr:uid="{00000000-0004-0000-0000-00003E010000}"/>
+    <hyperlink ref="C349" r:id="rId320" xr:uid="{00000000-0004-0000-0000-00003F010000}"/>
+    <hyperlink ref="C350" r:id="rId321" xr:uid="{00000000-0004-0000-0000-000040010000}"/>
+    <hyperlink ref="C351" r:id="rId322" xr:uid="{00000000-0004-0000-0000-000041010000}"/>
+    <hyperlink ref="C352" r:id="rId323" xr:uid="{00000000-0004-0000-0000-000042010000}"/>
+    <hyperlink ref="C353" r:id="rId324" xr:uid="{00000000-0004-0000-0000-000043010000}"/>
+    <hyperlink ref="C354" r:id="rId325" xr:uid="{00000000-0004-0000-0000-000044010000}"/>
+    <hyperlink ref="C358" r:id="rId326" xr:uid="{00000000-0004-0000-0000-000045010000}"/>
+    <hyperlink ref="C359" r:id="rId327" xr:uid="{00000000-0004-0000-0000-000046010000}"/>
+    <hyperlink ref="C360" r:id="rId328" xr:uid="{00000000-0004-0000-0000-000047010000}"/>
+    <hyperlink ref="C361" r:id="rId329" xr:uid="{00000000-0004-0000-0000-000048010000}"/>
+    <hyperlink ref="C362" r:id="rId330" xr:uid="{00000000-0004-0000-0000-000049010000}"/>
+    <hyperlink ref="C363" r:id="rId331" xr:uid="{00000000-0004-0000-0000-00004A010000}"/>
+    <hyperlink ref="C364" r:id="rId332" xr:uid="{00000000-0004-0000-0000-00004B010000}"/>
+    <hyperlink ref="C365" r:id="rId333" xr:uid="{00000000-0004-0000-0000-00004C010000}"/>
+    <hyperlink ref="C366" r:id="rId334" xr:uid="{00000000-0004-0000-0000-00004D010000}"/>
+    <hyperlink ref="C367" r:id="rId335" xr:uid="{00000000-0004-0000-0000-00004E010000}"/>
+    <hyperlink ref="C368" r:id="rId336" xr:uid="{00000000-0004-0000-0000-00004F010000}"/>
+    <hyperlink ref="C369" r:id="rId337" xr:uid="{00000000-0004-0000-0000-000050010000}"/>
+    <hyperlink ref="C370" r:id="rId338" xr:uid="{00000000-0004-0000-0000-000051010000}"/>
+    <hyperlink ref="C371" r:id="rId339" xr:uid="{00000000-0004-0000-0000-000052010000}"/>
+    <hyperlink ref="C372" r:id="rId340" xr:uid="{00000000-0004-0000-0000-000053010000}"/>
+    <hyperlink ref="C373" r:id="rId341" xr:uid="{00000000-0004-0000-0000-000054010000}"/>
+    <hyperlink ref="C374" r:id="rId342" xr:uid="{00000000-0004-0000-0000-000055010000}"/>
+    <hyperlink ref="C375" r:id="rId343" xr:uid="{00000000-0004-0000-0000-000056010000}"/>
+    <hyperlink ref="C376" r:id="rId344" xr:uid="{00000000-0004-0000-0000-000057010000}"/>
+    <hyperlink ref="C377" r:id="rId345" xr:uid="{00000000-0004-0000-0000-000058010000}"/>
+    <hyperlink ref="C378" r:id="rId346" xr:uid="{00000000-0004-0000-0000-000059010000}"/>
+    <hyperlink ref="C379" r:id="rId347" xr:uid="{00000000-0004-0000-0000-00005A010000}"/>
+    <hyperlink ref="C380" r:id="rId348" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color." xr:uid="{00000000-0004-0000-0000-00005B010000}"/>
+    <hyperlink ref="C381" r:id="rId349" xr:uid="{00000000-0004-0000-0000-00005C010000}"/>
+    <hyperlink ref="C382" r:id="rId350" xr:uid="{00000000-0004-0000-0000-00005D010000}"/>
+    <hyperlink ref="C383" r:id="rId351" xr:uid="{00000000-0004-0000-0000-00005E010000}"/>
+    <hyperlink ref="C384" r:id="rId352" xr:uid="{00000000-0004-0000-0000-00005F010000}"/>
+    <hyperlink ref="C385" r:id="rId353" xr:uid="{00000000-0004-0000-0000-000060010000}"/>
+    <hyperlink ref="C386" r:id="rId354" xr:uid="{00000000-0004-0000-0000-000061010000}"/>
+    <hyperlink ref="C387" r:id="rId355" xr:uid="{00000000-0004-0000-0000-000062010000}"/>
+    <hyperlink ref="C388" r:id="rId356" xr:uid="{00000000-0004-0000-0000-000063010000}"/>
+    <hyperlink ref="C389" r:id="rId357" xr:uid="{00000000-0004-0000-0000-000064010000}"/>
+    <hyperlink ref="C390" r:id="rId358" xr:uid="{00000000-0004-0000-0000-000065010000}"/>
+    <hyperlink ref="C391" r:id="rId359" xr:uid="{00000000-0004-0000-0000-000066010000}"/>
+    <hyperlink ref="C392" r:id="rId360" xr:uid="{00000000-0004-0000-0000-000067010000}"/>
+    <hyperlink ref="C393" r:id="rId361" xr:uid="{00000000-0004-0000-0000-000068010000}"/>
+    <hyperlink ref="C394" r:id="rId362" xr:uid="{00000000-0004-0000-0000-000069010000}"/>
+    <hyperlink ref="C395" r:id="rId363" xr:uid="{00000000-0004-0000-0000-00006A010000}"/>
+    <hyperlink ref="C397" r:id="rId364" xr:uid="{00000000-0004-0000-0000-00006B010000}"/>
+    <hyperlink ref="C396" r:id="rId365" xr:uid="{00000000-0004-0000-0000-00006C010000}"/>
+    <hyperlink ref="C398" r:id="rId366" xr:uid="{00000000-0004-0000-0000-00006D010000}"/>
+    <hyperlink ref="C399" r:id="rId367" xr:uid="{00000000-0004-0000-0000-00006E010000}"/>
+    <hyperlink ref="C400" r:id="rId368" xr:uid="{00000000-0004-0000-0000-00006F010000}"/>
+    <hyperlink ref="C403" r:id="rId369" xr:uid="{00000000-0004-0000-0000-000070010000}"/>
+    <hyperlink ref="C404" r:id="rId370" xr:uid="{00000000-0004-0000-0000-000071010000}"/>
+    <hyperlink ref="C405" r:id="rId371" xr:uid="{00000000-0004-0000-0000-000072010000}"/>
+    <hyperlink ref="C406" r:id="rId372" xr:uid="{00000000-0004-0000-0000-000073010000}"/>
+    <hyperlink ref="C407" r:id="rId373" xr:uid="{00000000-0004-0000-0000-000074010000}"/>
+    <hyperlink ref="C408" r:id="rId374" xr:uid="{00000000-0004-0000-0000-000075010000}"/>
+    <hyperlink ref="C411" r:id="rId375" xr:uid="{00000000-0004-0000-0000-000076010000}"/>
+    <hyperlink ref="C412" r:id="rId376" xr:uid="{00000000-0004-0000-0000-000077010000}"/>
+    <hyperlink ref="C413" r:id="rId377" xr:uid="{00000000-0004-0000-0000-000078010000}"/>
+    <hyperlink ref="C414" r:id="rId378" xr:uid="{00000000-0004-0000-0000-000079010000}"/>
+    <hyperlink ref="C415" r:id="rId379" xr:uid="{00000000-0004-0000-0000-00007A010000}"/>
+    <hyperlink ref="C416" r:id="rId380" xr:uid="{00000000-0004-0000-0000-00007B010000}"/>
+    <hyperlink ref="C417" r:id="rId381" xr:uid="{00000000-0004-0000-0000-00007C010000}"/>
+    <hyperlink ref="C418" r:id="rId382" xr:uid="{00000000-0004-0000-0000-00007D010000}"/>
+    <hyperlink ref="C419" r:id="rId383" xr:uid="{00000000-0004-0000-0000-00007E010000}"/>
+    <hyperlink ref="C420" r:id="rId384" xr:uid="{00000000-0004-0000-0000-00007F010000}"/>
+    <hyperlink ref="C421" r:id="rId385" xr:uid="{00000000-0004-0000-0000-000080010000}"/>
+    <hyperlink ref="C422" r:id="rId386" xr:uid="{00000000-0004-0000-0000-000081010000}"/>
+    <hyperlink ref="C423" r:id="rId387" xr:uid="{00000000-0004-0000-0000-000082010000}"/>
+    <hyperlink ref="C424" r:id="rId388" xr:uid="{00000000-0004-0000-0000-000083010000}"/>
+    <hyperlink ref="C425" r:id="rId389" xr:uid="{00000000-0004-0000-0000-000084010000}"/>
+    <hyperlink ref="C426" r:id="rId390" xr:uid="{00000000-0004-0000-0000-000085010000}"/>
+    <hyperlink ref="C427" r:id="rId391" xr:uid="{00000000-0004-0000-0000-000086010000}"/>
+    <hyperlink ref="C428" r:id="rId392" xr:uid="{00000000-0004-0000-0000-000087010000}"/>
+    <hyperlink ref="C429" r:id="rId393" xr:uid="{00000000-0004-0000-0000-000088010000}"/>
+    <hyperlink ref="C430" r:id="rId394" xr:uid="{00000000-0004-0000-0000-000089010000}"/>
+    <hyperlink ref="C431" r:id="rId395" xr:uid="{00000000-0004-0000-0000-00008A010000}"/>
+    <hyperlink ref="C432" r:id="rId396" xr:uid="{00000000-0004-0000-0000-00008B010000}"/>
+    <hyperlink ref="C433" r:id="rId397" xr:uid="{00000000-0004-0000-0000-00008C010000}"/>
+    <hyperlink ref="C434" r:id="rId398" xr:uid="{00000000-0004-0000-0000-00008D010000}"/>
+    <hyperlink ref="C435" r:id="rId399" xr:uid="{00000000-0004-0000-0000-00008E010000}"/>
+    <hyperlink ref="C436" r:id="rId400" xr:uid="{00000000-0004-0000-0000-00008F010000}"/>
+    <hyperlink ref="C437" r:id="rId401" xr:uid="{00000000-0004-0000-0000-000090010000}"/>
+    <hyperlink ref="C438" r:id="rId402" xr:uid="{00000000-0004-0000-0000-000091010000}"/>
+    <hyperlink ref="C439" r:id="rId403" xr:uid="{00000000-0004-0000-0000-000092010000}"/>
+    <hyperlink ref="C440" r:id="rId404" xr:uid="{00000000-0004-0000-0000-000093010000}"/>
+    <hyperlink ref="C441" r:id="rId405" xr:uid="{00000000-0004-0000-0000-000094010000}"/>
+    <hyperlink ref="C442" r:id="rId406" xr:uid="{00000000-0004-0000-0000-000095010000}"/>
+    <hyperlink ref="C443" r:id="rId407" xr:uid="{00000000-0004-0000-0000-000096010000}"/>
+    <hyperlink ref="C444" r:id="rId408" xr:uid="{00000000-0004-0000-0000-000097010000}"/>
+    <hyperlink ref="C445" r:id="rId409" xr:uid="{00000000-0004-0000-0000-000098010000}"/>
+    <hyperlink ref="C446" r:id="rId410" xr:uid="{00000000-0004-0000-0000-000099010000}"/>
+    <hyperlink ref="C447" r:id="rId411" xr:uid="{00000000-0004-0000-0000-00009A010000}"/>
+    <hyperlink ref="C448" r:id="rId412" xr:uid="{00000000-0004-0000-0000-00009B010000}"/>
+    <hyperlink ref="C449" r:id="rId413" xr:uid="{00000000-0004-0000-0000-00009C010000}"/>
+    <hyperlink ref="C450" r:id="rId414" xr:uid="{00000000-0004-0000-0000-00009D010000}"/>
+    <hyperlink ref="C452" r:id="rId415" xr:uid="{00000000-0004-0000-0000-00009E010000}"/>
+    <hyperlink ref="C451" r:id="rId416" xr:uid="{00000000-0004-0000-0000-00009F010000}"/>
+    <hyperlink ref="C453" r:id="rId417" xr:uid="{00000000-0004-0000-0000-0000A0010000}"/>
+    <hyperlink ref="C454" r:id="rId418" xr:uid="{00000000-0004-0000-0000-0000A1010000}"/>
+    <hyperlink ref="C455" r:id="rId419" xr:uid="{00000000-0004-0000-0000-0000A2010000}"/>
+    <hyperlink ref="C456" r:id="rId420" xr:uid="{00000000-0004-0000-0000-0000A3010000}"/>
+    <hyperlink ref="C457" r:id="rId421" xr:uid="{00000000-0004-0000-0000-0000A4010000}"/>
+    <hyperlink ref="C458" r:id="rId422" xr:uid="{00000000-0004-0000-0000-0000A5010000}"/>
+    <hyperlink ref="C459" r:id="rId423" xr:uid="{00000000-0004-0000-0000-0000A6010000}"/>
+    <hyperlink ref="C460" r:id="rId424" xr:uid="{00000000-0004-0000-0000-0000A7010000}"/>
+    <hyperlink ref="C461" r:id="rId425" xr:uid="{00000000-0004-0000-0000-0000A8010000}"/>
+    <hyperlink ref="C462" r:id="rId426" xr:uid="{00000000-0004-0000-0000-0000A9010000}"/>
+    <hyperlink ref="C463" r:id="rId427" xr:uid="{00000000-0004-0000-0000-0000AA010000}"/>
+    <hyperlink ref="C470" r:id="rId428" xr:uid="{00000000-0004-0000-0000-0000AB010000}"/>
+    <hyperlink ref="C469" r:id="rId429" xr:uid="{00000000-0004-0000-0000-0000AC010000}"/>
+    <hyperlink ref="C468" r:id="rId430" xr:uid="{00000000-0004-0000-0000-0000AD010000}"/>
+    <hyperlink ref="C467" r:id="rId431" xr:uid="{00000000-0004-0000-0000-0000AE010000}"/>
+    <hyperlink ref="C466" r:id="rId432" xr:uid="{00000000-0004-0000-0000-0000AF010000}"/>
+    <hyperlink ref="C465" r:id="rId433" xr:uid="{00000000-0004-0000-0000-0000B0010000}"/>
+    <hyperlink ref="C464" r:id="rId434" xr:uid="{00000000-0004-0000-0000-0000B1010000}"/>
+    <hyperlink ref="C473" r:id="rId435" xr:uid="{00000000-0004-0000-0000-0000B2010000}"/>
+    <hyperlink ref="C474" r:id="rId436" xr:uid="{00000000-0004-0000-0000-0000B3010000}"/>
+    <hyperlink ref="C475" r:id="rId437" xr:uid="{00000000-0004-0000-0000-0000B4010000}"/>
+    <hyperlink ref="C476" r:id="rId438" xr:uid="{00000000-0004-0000-0000-0000B5010000}"/>
+    <hyperlink ref="C477" r:id="rId439" xr:uid="{00000000-0004-0000-0000-0000B6010000}"/>
+    <hyperlink ref="C478" r:id="rId440" xr:uid="{00000000-0004-0000-0000-0000B7010000}"/>
+    <hyperlink ref="C479" r:id="rId441" xr:uid="{00000000-0004-0000-0000-0000B8010000}"/>
+    <hyperlink ref="C482" r:id="rId442" xr:uid="{00000000-0004-0000-0000-0000B9010000}"/>
+    <hyperlink ref="C480" r:id="rId443" xr:uid="{00000000-0004-0000-0000-0000BA010000}"/>
+    <hyperlink ref="C481" r:id="rId444" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{00000000-0004-0000-0000-0000BB010000}"/>
+    <hyperlink ref="C357" r:id="rId445" xr:uid="{00000000-0004-0000-0000-0000BC010000}"/>
+    <hyperlink ref="C9" r:id="rId446" xr:uid="{00000000-0004-0000-0000-0000BD010000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId447"/>

</xml_diff>